<commit_message>
Updated BOM of D20V15, Added D6V4 and PD6V3
</commit_message>
<xml_diff>
--- a/Dice/D20/D20v15/D20V15 BOM.xlsx
+++ b/Dice/D20/D20v15/D20V15 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Pixels-dice\Electrical\Dice\D20\D20v15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A2CCC42-83DF-44EB-B203-23DD3C95857A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4421385-7EA8-40DB-8A72-D59BC84B775E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16965" yWindow="780" windowWidth="20910" windowHeight="18555"/>
+    <workbookView xWindow="26025" yWindow="3990" windowWidth="23475" windowHeight="14670"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="143">
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>C:\Projects\Pixels-dice\Electrical\Dice\D20\D20v15\Main.kicad_sch</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
   <si>
     <t>Item</t>
   </si>
@@ -64,54 +73,72 @@
     <t>MGMA3216H2450-A02</t>
   </si>
   <si>
+    <t>C1, C4, C18</t>
+  </si>
+  <si>
+    <t>4.7uF 10V 20%</t>
+  </si>
+  <si>
+    <t>Pixels-dice:C_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>GRM155R61A475MEAAJ</t>
+  </si>
+  <si>
+    <t>C2, C5</t>
+  </si>
+  <si>
+    <t>8pF 10V 10%</t>
+  </si>
+  <si>
+    <t>GRT1555C2A8R0DA02</t>
+  </si>
+  <si>
+    <t>C3, C10, C23, C24, C25</t>
+  </si>
+  <si>
+    <t>0.1uF 10V 20%</t>
+  </si>
+  <si>
+    <t>GRM155R61H104KE19D</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>100pF NP0 10V 5%</t>
+  </si>
+  <si>
+    <t>GCM1555C1H101JA16J</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>0.8pF 10V 5% C0G</t>
+  </si>
+  <si>
+    <t>Pixels-dice:0402_RF</t>
+  </si>
+  <si>
+    <t>GJM1555C1HR80BB01</t>
+  </si>
+  <si>
+    <t>C9, C16</t>
+  </si>
+  <si>
     <t>10uF 10V 20%</t>
   </si>
   <si>
-    <t>Pixels-dice:C_0402_1005Metric</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Murata</t>
-  </si>
-  <si>
     <t>GRM155R61A106ME11D</t>
   </si>
   <si>
-    <t>8pF 10V 10%</t>
-  </si>
-  <si>
-    <t>GRT1555C2A8R0DA02</t>
-  </si>
-  <si>
-    <t>0.1uF 10V 20%</t>
-  </si>
-  <si>
-    <t>GRM155R61H104KE19D</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>100pF NP0 10V 5%</t>
-  </si>
-  <si>
-    <t>GCM1555C1H101JA16J</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>0.8pF 10V 5% C0G</t>
-  </si>
-  <si>
-    <t>Pixels-dice:0402_RF</t>
-  </si>
-  <si>
-    <t>GJM1555C1HR80BB01</t>
-  </si>
-  <si>
     <t>C12</t>
   </si>
   <si>
@@ -139,7 +166,7 @@
     <t>22uF 10V 20%</t>
   </si>
   <si>
-    <t>ZRB18AR61A226ME01L</t>
+    <t>GRM188R61A226ME15D</t>
   </si>
   <si>
     <t>C19</t>
@@ -154,6 +181,9 @@
     <t>GRM3195C1H333JA01J</t>
   </si>
   <si>
+    <t>C21, C22</t>
+  </si>
+  <si>
     <t>10nF 25V 10%</t>
   </si>
   <si>
@@ -175,6 +205,9 @@
     <t>BAV99S,115</t>
   </si>
   <si>
+    <t>D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15, D16, D17, D18, D19, D20, D21</t>
+  </si>
+  <si>
     <t>TX1812Z_2020</t>
   </si>
   <si>
@@ -229,6 +262,9 @@
     <t>LQG15HS3N9B02D</t>
   </si>
   <si>
+    <t>R1, R2, R7</t>
+  </si>
+  <si>
     <t>4.02M 1%</t>
   </si>
   <si>
@@ -250,6 +286,9 @@
     <t>0402WGJ0103TCE</t>
   </si>
   <si>
+    <t>R4, R5, R9, R10</t>
+  </si>
+  <si>
     <t>100k 1%</t>
   </si>
   <si>
@@ -274,6 +313,9 @@
     <t>0402WGF1005TCE</t>
   </si>
   <si>
+    <t>R12, R16</t>
+  </si>
+  <si>
     <t>2.7k 5%</t>
   </si>
   <si>
@@ -407,30 +449,6 @@
   </si>
   <si>
     <t>XRCGB32M000F2P00R0</t>
-  </si>
-  <si>
-    <t>C1, C4, C9, C16, C18</t>
-  </si>
-  <si>
-    <t>C2, C5</t>
-  </si>
-  <si>
-    <t>C3, C6, C10, C23, C24, C25</t>
-  </si>
-  <si>
-    <t>C21, C22</t>
-  </si>
-  <si>
-    <t>D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15, D16, D17, D18, D19, D20, D21</t>
-  </si>
-  <si>
-    <t>R1, R2, R7</t>
-  </si>
-  <si>
-    <t>R4, R5, R9, R10</t>
-  </si>
-  <si>
-    <t>R12, R16</t>
   </si>
 </sst>
 </file>
@@ -931,15 +949,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1295,718 +1308,656 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B2" s="1">
+        <v>44911.901932870373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H5" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
         <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
+      <c r="C9" t="s">
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>37</v>
+      <c r="C10" t="s">
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
         <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>132</v>
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>47</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" t="s">
         <v>48</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>55</v>
+      <c r="C15" t="s">
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>59</v>
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>63</v>
+      <c r="C17" t="s">
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>134</v>
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
       </c>
       <c r="D19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" t="s">
         <v>69</v>
-      </c>
-      <c r="E19" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" t="s">
         <v>73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>135</v>
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>74</v>
       </c>
       <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" t="s">
         <v>76</v>
-      </c>
-      <c r="E21" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
         <v>78</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
         <v>79</v>
-      </c>
-      <c r="E22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" t="s">
         <v>81</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>82</v>
       </c>
-      <c r="E23" t="s">
-        <v>70</v>
-      </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G23" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>136</v>
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="H24" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>86</v>
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>90</v>
+      <c r="C26" t="s">
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G26" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" t="s">
         <v>93</v>
-      </c>
-      <c r="H26" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s">
         <v>95</v>
       </c>
-      <c r="D27" t="s">
-        <v>96</v>
-      </c>
       <c r="E27" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G27" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="H27" t="s">
         <v>96</v>
@@ -2014,184 +1965,288 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" t="s">
         <v>99</v>
-      </c>
-      <c r="D28" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" t="s">
-        <v>101</v>
-      </c>
-      <c r="F28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" t="s">
-        <v>102</v>
-      </c>
-      <c r="H28" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" t="s">
         <v>103</v>
-      </c>
-      <c r="D29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" t="s">
-        <v>105</v>
-      </c>
-      <c r="F29" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" t="s">
-        <v>106</v>
-      </c>
-      <c r="H29" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
+        <v>107</v>
+      </c>
+      <c r="H30" t="s">
         <v>108</v>
-      </c>
-      <c r="D30" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" t="s">
-        <v>110</v>
-      </c>
-      <c r="F30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" t="s">
-        <v>111</v>
-      </c>
-      <c r="H30" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
         <v>112</v>
       </c>
-      <c r="D31" t="s">
-        <v>113</v>
-      </c>
-      <c r="E31" t="s">
-        <v>105</v>
-      </c>
-      <c r="F31" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" t="s">
-        <v>114</v>
-      </c>
       <c r="H31" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" t="s">
         <v>115</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
         <v>116</v>
       </c>
-      <c r="E32" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" t="s">
-        <v>118</v>
-      </c>
       <c r="H32" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" t="s">
+        <v>119</v>
+      </c>
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" t="s">
         <v>120</v>
       </c>
-      <c r="D33" t="s">
+      <c r="H33" t="s">
         <v>121</v>
-      </c>
-      <c r="E33" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" t="s">
-        <v>123</v>
-      </c>
-      <c r="H33" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
         <v>125</v>
       </c>
-      <c r="D34" t="s">
+      <c r="H34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
         <v>126</v>
       </c>
-      <c r="E34" t="s">
+      <c r="D35" t="s">
         <v>127</v>
       </c>
-      <c r="F34" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="E35" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
         <v>128</v>
+      </c>
+      <c r="H35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" t="s">
+        <v>130</v>
+      </c>
+      <c r="E36" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" t="s">
+        <v>132</v>
+      </c>
+      <c r="H36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D37" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" t="s">
+        <v>137</v>
+      </c>
+      <c r="H37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>57</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D38" t="s">
+        <v>140</v>
+      </c>
+      <c r="E38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>